<commit_message>
Add creating invoice (window, exceptions, logic)
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\InvoiceRegister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AEF5AC-6392-4859-82FE-BBEB8774ECD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134769AC-B232-4170-9CB2-A87145448264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E493C55E-29D7-4918-BC32-7906BFE9D56E}"/>
   </bookViews>
@@ -589,7 +589,7 @@
   <dimension ref="B2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +601,8 @@
     <col min="6" max="6" width="30.5703125" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.140625" customWidth="1"/>
     <col min="12" max="12" width="4.85546875" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" customWidth="1"/>
@@ -650,7 +651,7 @@
       <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="M3" t="s">
@@ -676,7 +677,7 @@
       <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="M4" t="s">
@@ -702,7 +703,7 @@
       <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M5" t="s">
@@ -725,7 +726,7 @@
       <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M6" t="s">
@@ -745,7 +746,7 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add initial implementation of creating items
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\InvoiceRegister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134769AC-B232-4170-9CB2-A87145448264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C595BA-741B-402C-8E1D-EEF323CB5FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E493C55E-29D7-4918-BC32-7906BFE9D56E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>InvoiceNumber</t>
   </si>
@@ -93,9 +93,6 @@
     <t>InvoiceItem</t>
   </si>
   <si>
-    <t>Edit</t>
-  </si>
-  <si>
     <t>Delete</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Filter</t>
   </si>
   <si>
-    <t>EditItem</t>
-  </si>
-  <si>
     <t>DeleteItem</t>
   </si>
   <si>
@@ -205,6 +199,12 @@
   </si>
   <si>
     <t>Send warning mail</t>
+  </si>
+  <si>
+    <t>ClientEmail</t>
+  </si>
+  <si>
+    <t>PriceGross</t>
   </si>
 </sst>
 </file>
@@ -230,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +249,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -262,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -272,6 +278,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -586,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F738C2-135B-4D7D-B142-13F9B89CFB3E}">
-  <dimension ref="B2:Q34"/>
+  <dimension ref="B2:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,65 +620,65 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="4"/>
       <c r="H2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N2" s="4"/>
       <c r="P2" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
@@ -681,23 +688,23 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
@@ -707,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -717,10 +724,10 @@
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H6" t="s">
@@ -730,7 +737,7 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -740,10 +747,10 @@
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -757,10 +764,10 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -771,10 +778,10 @@
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -785,10 +792,10 @@
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -799,11 +806,11 @@
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
@@ -813,10 +820,10 @@
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -827,97 +834,106 @@
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" t="s">
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>26</v>
+      <c r="E19" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -925,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s">
         <v>18</v>
@@ -944,7 +960,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
@@ -979,17 +995,12 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E32" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add creating, deleting InvoiceItems
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\InvoiceRegister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233592DE-2E6F-4A58-A4FD-6B0BE1076C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286866F1-4C01-4C1A-8B2E-3FBE8B9A390F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E493C55E-29D7-4918-BC32-7906BFE9D56E}"/>
   </bookViews>
@@ -230,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,12 +246,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,10 +269,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -595,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F738C2-135B-4D7D-B142-13F9B89CFB3E}">
   <dimension ref="B2:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -619,28 +613,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="4"/>
       <c r="H2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="P2" s="5" t="s">
+      <c r="N2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -655,7 +649,7 @@
       <c r="F3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -681,7 +675,7 @@
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -707,7 +701,7 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -730,7 +724,7 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -864,10 +858,10 @@
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -891,7 +885,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -907,7 +901,7 @@
       <c r="B21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -920,10 +914,10 @@
       <c r="B23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
@@ -940,10 +934,10 @@
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -951,10 +945,10 @@
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -962,34 +956,34 @@
       <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -999,7 +993,7 @@
       </c>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add emailsender and appsettings.json
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\InvoiceRegister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1EE13F-5A58-48AC-A000-EE3F7EF123EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAFFD60-40CD-4EE4-ABA3-22CB95EB8395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="90" windowWidth="29040" windowHeight="15720" xr2:uid="{E493C55E-29D7-4918-BC32-7906BFE9D56E}"/>
   </bookViews>
@@ -222,7 +222,7 @@
     <t>Apply filter on refresh</t>
   </si>
   <si>
-    <t>Database cloud</t>
+    <t>Przygotować liste funkcjonalnosci</t>
   </si>
 </sst>
 </file>
@@ -604,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F738C2-135B-4D7D-B142-13F9B89CFB3E}">
-  <dimension ref="B2:T36"/>
+  <dimension ref="B2:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.140625" customWidth="1"/>
     <col min="12" max="12" width="4.85546875" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="13" max="13" width="39.85546875" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="15" max="15" width="6.85546875" customWidth="1"/>
     <col min="16" max="16" width="23.28515625" customWidth="1"/>
@@ -678,7 +678,7 @@
         <v>50</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>31</v>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>60</v>
@@ -759,9 +759,9 @@
         <v>2</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -781,6 +781,9 @@
       <c r="K7" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="M7" t="s">
+        <v>62</v>
+      </c>
       <c r="P7" t="s">
         <v>59</v>
       </c>
@@ -798,9 +801,6 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P8" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -901,7 +901,6 @@
       <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1030,16 +1029,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Add small changes on email content
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\InvoiceRegister\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFEC832-9B85-4684-8E4C-5F4F4581AF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC32D6A-2BB5-4636-80D8-9E1AC3024443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="90" windowWidth="29040" windowHeight="15720" xr2:uid="{E493C55E-29D7-4918-BC32-7906BFE9D56E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
   <si>
     <t>InvoiceNumber</t>
   </si>
@@ -241,6 +241,45 @@
   </si>
   <si>
     <t>Zmiana statusu faktury</t>
+  </si>
+  <si>
+    <t>Wykorzystane technologie</t>
+  </si>
+  <si>
+    <t>Entity Framework</t>
+  </si>
+  <si>
+    <t>MSSQL</t>
+  </si>
+  <si>
+    <t>.NET WPF</t>
+  </si>
+  <si>
+    <t>SendGrid (EmailSender)</t>
+  </si>
+  <si>
+    <t>PdfSharp (PdfGenerator)</t>
+  </si>
+  <si>
+    <t>AutoMapper</t>
+  </si>
+  <si>
+    <t>Dependency Injection</t>
+  </si>
+  <si>
+    <t>Wzorce projektowe i architektura</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>Factory</t>
+  </si>
+  <si>
+    <t>Microservices</t>
+  </si>
+  <si>
+    <t>MVVM</t>
   </si>
 </sst>
 </file>
@@ -298,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -308,7 +347,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -675,7 +713,7 @@
   <dimension ref="B2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,13 +749,13 @@
       <c r="J2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -960,6 +998,9 @@
       <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="P14" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
@@ -971,6 +1012,9 @@
       <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="P15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -982,8 +1026,11 @@
       <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
@@ -993,29 +1040,41 @@
       <c r="F17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1023,12 +1082,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1036,8 +1098,11 @@
         <v>45</v>
       </c>
       <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1047,8 +1112,11 @@
       <c r="F24" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1058,8 +1126,11 @@
       <c r="F25" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1069,8 +1140,11 @@
       <c r="F26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1080,8 +1154,11 @@
       <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
@@ -1097,7 +1174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
@@ -1105,7 +1182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E32" s="3" t="s">
         <v>20</v>
       </c>

</xml_diff>